<commit_message>
added yellow color for status
</commit_message>
<xml_diff>
--- a/Подробный отчет.xlsx
+++ b/Подробный отчет.xlsx
@@ -35,7 +35,7 @@
       <sz val="16"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -46,6 +46,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
         <bgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -90,11 +96,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>

</xml_diff>